<commit_message>
Updated files for replication
</commit_message>
<xml_diff>
--- a/999_Replication_Paper/01_Basel_I/Basel_I_Algo_Data.xlsx
+++ b/999_Replication_Paper/01_Basel_I/Basel_I_Algo_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colliard\Desktop\Measuring Regulatory Complexity\Basel I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colliard\Desktop\RegulatoryComplexity_Replication\01_Basel_I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F0597-6C43-40BA-87BA-C7E81617C1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF62F3-06C8-437F-9A86-6095401A59E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>4a</t>
   </si>
@@ -109,6 +109,195 @@
   </si>
   <si>
     <t>WORD INDEX</t>
+  </si>
+  <si>
+    <t>WORD</t>
+  </si>
+  <si>
+    <t>“=”</t>
+  </si>
+  <si>
+    <t>“==”</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>ELSE</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>!=</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>AfDB</t>
+  </si>
+  <si>
+    <t>AsDB</t>
+  </si>
+  <si>
+    <t>ASSET_CLASS</t>
+  </si>
+  <si>
+    <t>ASSET_MATURITY</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>banks</t>
+  </si>
+  <si>
+    <t>capital</t>
+  </si>
+  <si>
+    <t>capital_instruments</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>CASH_COLLECTION</t>
+  </si>
+  <si>
+    <t>central_banks</t>
+  </si>
+  <si>
+    <t>central_governments</t>
+  </si>
+  <si>
+    <t>claims</t>
+  </si>
+  <si>
+    <t>COLLATERALIZED</t>
+  </si>
+  <si>
+    <t>commercial_companies</t>
+  </si>
+  <si>
+    <t>DEDUCTED_FROM</t>
+  </si>
+  <si>
+    <t>DENOMINATION</t>
+  </si>
+  <si>
+    <t>domestic</t>
+  </si>
+  <si>
+    <t>EIB</t>
+  </si>
+  <si>
+    <t>entities</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>FUNDING_CURRENCY</t>
+  </si>
+  <si>
+    <t>GUARANTEED</t>
+  </si>
+  <si>
+    <t>GUARANTEED_COUNTRY</t>
+  </si>
+  <si>
+    <t>IADB</t>
+  </si>
+  <si>
+    <t>IBRD</t>
+  </si>
+  <si>
+    <t>in_process</t>
+  </si>
+  <si>
+    <t>ISSUER</t>
+  </si>
+  <si>
+    <t>ISSUER_COUNTRY</t>
+  </si>
+  <si>
+    <t>ISSUER_OWNER</t>
+  </si>
+  <si>
+    <t>LOAN_SECURITY</t>
+  </si>
+  <si>
+    <t>loans</t>
+  </si>
+  <si>
+    <t>mortgage</t>
+  </si>
+  <si>
+    <t>national</t>
+  </si>
+  <si>
+    <t>national_discretion</t>
+  </si>
+  <si>
+    <t>oecd</t>
+  </si>
+  <si>
+    <t>other_fixed_assets</t>
+  </si>
+  <si>
+    <t>other_investments</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>premises</t>
+  </si>
+  <si>
+    <t>private_sector</t>
+  </si>
+  <si>
+    <t>PROPERTY_OCCUPIED</t>
+  </si>
+  <si>
+    <t>public_sector</t>
+  </si>
+  <si>
+    <t>public-sector_entities</t>
+  </si>
+  <si>
+    <t>real_estate</t>
+  </si>
+  <si>
+    <t>rented</t>
+  </si>
+  <si>
+    <t>risk_weight</t>
+  </si>
+  <si>
+    <t>THEN:</t>
   </si>
 </sst>
 </file>
@@ -144,8 +333,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,97 +720,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B0CC2F-EC12-4DA2-98A6-D6AB776C81A3}">
-  <dimension ref="A1:Y64"/>
+  <dimension ref="A1:Z64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
-        <v>0</v>
-      </c>
       <c r="Q1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
         <v>2</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>3</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>4</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>5</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>6</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>7</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -627,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -687,60 +886,63 @@
         <v>1</v>
       </c>
       <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>4</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>3</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>8</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>16</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>6</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>4</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>6</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>4</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -749,116 +951,122 @@
         <v>2</v>
       </c>
       <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
         <v>3</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>4</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
       </c>
       <c r="W3">
         <v>2</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <v>8</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>4</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>8</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
       <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>2</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
       <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
         <v>3</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>4</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>2</v>
       </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
       <c r="V4">
         <v>0</v>
       </c>
       <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>2</v>
       </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
       <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -915,30 +1123,33 @@
         <v>0</v>
       </c>
       <c r="X5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="Z5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -992,33 +1203,36 @@
         <v>1</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1030,11 +1244,11 @@
         <v>1</v>
       </c>
       <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
         <v>14</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
       <c r="M7">
         <v>1</v>
       </c>
@@ -1042,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1060,30 +1274,33 @@
         <v>0</v>
       </c>
       <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>4</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>2</v>
       </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1113,11 +1330,11 @@
         <v>0</v>
       </c>
       <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <v>2</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
       <c r="O8">
         <v>0</v>
       </c>
@@ -1128,10 +1345,10 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1149,21 +1366,24 @@
         <v>0</v>
       </c>
       <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1181,23 +1401,23 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
         <v>4</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
       <c r="P9">
         <v>0</v>
       </c>
@@ -1205,14 +1425,14 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
         <v>3</v>
       </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
       <c r="U9">
         <v>0</v>
       </c>
@@ -1220,27 +1440,30 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1267,11 +1490,11 @@
         <v>0</v>
       </c>
       <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <v>2</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
       <c r="O10">
         <v>0</v>
       </c>
@@ -1303,21 +1526,24 @@
         <v>0</v>
       </c>
       <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1359,10 +1585,10 @@
         <v>0</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -1380,18 +1606,21 @@
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1400,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1412,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1457,18 +1686,21 @@
         <v>0</v>
       </c>
       <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A13">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1492,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1507,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1534,18 +1766,21 @@
         <v>0</v>
       </c>
       <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A14">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1584,10 +1819,10 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -1611,18 +1846,21 @@
         <v>0</v>
       </c>
       <c r="Y14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1664,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -1688,18 +1926,21 @@
         <v>1</v>
       </c>
       <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A16">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1723,11 +1964,11 @@
         <v>0</v>
       </c>
       <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>3</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
       <c r="M16">
         <v>0</v>
       </c>
@@ -1765,18 +2006,21 @@
         <v>0</v>
       </c>
       <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A17">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1800,11 +2044,11 @@
         <v>0</v>
       </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>3</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
       <c r="M17">
         <v>0</v>
       </c>
@@ -1842,18 +2086,21 @@
         <v>0</v>
       </c>
       <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A18">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1862,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1874,13 +2121,13 @@
         <v>1</v>
       </c>
       <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
         <v>2</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
       <c r="L18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M18">
         <v>2</v>
@@ -1889,7 +2136,7 @@
         <v>2</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P18">
         <v>1</v>
@@ -1907,30 +2154,33 @@
         <v>1</v>
       </c>
       <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
         <v>4</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>2</v>
       </c>
-      <c r="W18">
-        <v>1</v>
-      </c>
       <c r="X18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A19">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1960,11 +2210,11 @@
         <v>0</v>
       </c>
       <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
         <v>2</v>
       </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
       <c r="O19">
         <v>0</v>
       </c>
@@ -1975,10 +2225,10 @@
         <v>0</v>
       </c>
       <c r="R19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19">
         <v>0</v>
@@ -1996,18 +2246,21 @@
         <v>0</v>
       </c>
       <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A20">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2034,14 +2287,14 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
         <v>2</v>
       </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
       <c r="O20">
         <v>0</v>
       </c>
@@ -2073,18 +2326,21 @@
         <v>0</v>
       </c>
       <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A21">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2129,10 +2385,10 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -2144,24 +2400,27 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A22">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2221,24 +2480,27 @@
         <v>0</v>
       </c>
       <c r="W22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2298,24 +2560,27 @@
         <v>0</v>
       </c>
       <c r="W23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2324,10 +2589,10 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2351,10 +2616,10 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -2381,18 +2646,21 @@
         <v>0</v>
       </c>
       <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2428,10 +2696,10 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -2458,18 +2726,21 @@
         <v>0</v>
       </c>
       <c r="Y25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2481,13 +2752,13 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -2535,18 +2806,21 @@
         <v>0</v>
       </c>
       <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A27">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2558,20 +2832,20 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
         <v>2</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
       <c r="L27">
         <v>0</v>
       </c>
@@ -2579,11 +2853,11 @@
         <v>0</v>
       </c>
       <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
         <v>2</v>
       </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
       <c r="P27">
         <v>0</v>
       </c>
@@ -2612,18 +2886,21 @@
         <v>0</v>
       </c>
       <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A28">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2635,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2650,22 +2927,22 @@
         <v>1</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28">
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28">
         <v>1</v>
@@ -2677,7 +2954,7 @@
         <v>1</v>
       </c>
       <c r="U28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28">
         <v>0</v>
@@ -2689,18 +2966,21 @@
         <v>0</v>
       </c>
       <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A29">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2718,17 +2998,17 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
         <v>5</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
       <c r="M29">
         <v>0</v>
       </c>
@@ -2766,18 +3046,21 @@
         <v>0</v>
       </c>
       <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A30">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2828,10 +3111,10 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -2843,18 +3126,21 @@
         <v>0</v>
       </c>
       <c r="Y30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2914,24 +3200,27 @@
         <v>0</v>
       </c>
       <c r="W31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2943,10 +3232,10 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2979,10 +3268,10 @@
         <v>0</v>
       </c>
       <c r="S32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32">
         <v>0</v>
@@ -2997,18 +3286,21 @@
         <v>0</v>
       </c>
       <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A33">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33">
         <v>32</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -3029,11 +3321,11 @@
         <v>0</v>
       </c>
       <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
         <v>4</v>
       </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
       <c r="L33">
         <v>0</v>
       </c>
@@ -3041,11 +3333,11 @@
         <v>0</v>
       </c>
       <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
         <v>2</v>
       </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
       <c r="P33">
         <v>0</v>
       </c>
@@ -3074,18 +3366,21 @@
         <v>0</v>
       </c>
       <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A34">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -3109,11 +3404,11 @@
         <v>0</v>
       </c>
       <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
         <v>3</v>
       </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
       <c r="M34">
         <v>0</v>
       </c>
@@ -3151,18 +3446,21 @@
         <v>0</v>
       </c>
       <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35">
         <v>34</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -3230,16 +3528,19 @@
       <c r="Y35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A36">
+      <c r="Z35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36">
         <v>35</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -3293,10 +3594,10 @@
         <v>0</v>
       </c>
       <c r="U36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W36">
         <v>0</v>
@@ -3305,18 +3606,21 @@
         <v>0</v>
       </c>
       <c r="Y36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37">
         <v>36</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -3328,10 +3632,10 @@
         <v>0</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -3364,10 +3668,10 @@
         <v>0</v>
       </c>
       <c r="S37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U37">
         <v>0</v>
@@ -3382,18 +3686,21 @@
         <v>0</v>
       </c>
       <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A38">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38">
         <v>37</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -3411,26 +3718,26 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
         <v>2</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>5</v>
       </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
       <c r="M38">
         <v>1</v>
       </c>
       <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
         <v>2</v>
       </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
       <c r="P38">
         <v>0</v>
       </c>
@@ -3459,18 +3766,21 @@
         <v>0</v>
       </c>
       <c r="Y38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A39">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39">
         <v>38</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -3491,23 +3801,23 @@
         <v>0</v>
       </c>
       <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
         <v>2</v>
       </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
       <c r="L39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39">
         <v>1</v>
       </c>
       <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
         <v>2</v>
       </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
       <c r="P39">
         <v>0</v>
       </c>
@@ -3536,18 +3846,21 @@
         <v>0</v>
       </c>
       <c r="Y39">
+        <v>0</v>
+      </c>
+      <c r="Z39">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A40">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40">
         <v>39</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -3571,11 +3884,11 @@
         <v>0</v>
       </c>
       <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
         <v>3</v>
       </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
       <c r="M40">
         <v>0</v>
       </c>
@@ -3613,18 +3926,21 @@
         <v>0</v>
       </c>
       <c r="Y40">
+        <v>0</v>
+      </c>
+      <c r="Z40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A41">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41">
         <v>40</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -3648,11 +3964,11 @@
         <v>0</v>
       </c>
       <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
         <v>3</v>
       </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
       <c r="M41">
         <v>0</v>
       </c>
@@ -3690,18 +4006,21 @@
         <v>0</v>
       </c>
       <c r="Y41">
+        <v>0</v>
+      </c>
+      <c r="Z41">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42">
         <v>41</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -3737,10 +4056,10 @@
         <v>0</v>
       </c>
       <c r="O42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q42">
         <v>0</v>
@@ -3767,18 +4086,21 @@
         <v>0</v>
       </c>
       <c r="Y42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43">
         <v>42</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -3790,37 +4112,37 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H43">
         <v>2</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
         <v>2</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>5</v>
       </c>
-      <c r="L43">
-        <v>1</v>
-      </c>
       <c r="M43">
         <v>1</v>
       </c>
       <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
         <v>2</v>
       </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
       <c r="P43">
         <v>0</v>
       </c>
       <c r="Q43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R43">
         <v>1</v>
@@ -3832,30 +4154,33 @@
         <v>1</v>
       </c>
       <c r="U43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V43">
         <v>0</v>
       </c>
       <c r="W43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y43">
+        <v>0</v>
+      </c>
+      <c r="Z43">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A44">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44">
         <v>43</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -3870,29 +4195,29 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
         <v>2</v>
       </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
       <c r="L44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44">
         <v>1</v>
       </c>
       <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44">
         <v>2</v>
       </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
       <c r="P44">
         <v>0</v>
       </c>
@@ -3900,13 +4225,13 @@
         <v>0</v>
       </c>
       <c r="R44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S44">
         <v>1</v>
       </c>
       <c r="T44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U44">
         <v>0</v>
@@ -3921,18 +4246,21 @@
         <v>0</v>
       </c>
       <c r="Y44">
+        <v>0</v>
+      </c>
+      <c r="Z44">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A45">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45">
         <v>44</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -3983,10 +4311,10 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V45">
         <v>0</v>
@@ -3998,18 +4326,21 @@
         <v>0</v>
       </c>
       <c r="Y45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46">
         <v>45</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -4048,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="P46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46">
         <v>0</v>
@@ -4075,18 +4406,21 @@
         <v>0</v>
       </c>
       <c r="Y46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47">
         <v>46</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -4107,13 +4441,13 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M47">
         <v>1</v>
@@ -4122,13 +4456,13 @@
         <v>1</v>
       </c>
       <c r="O47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47">
         <v>0</v>
@@ -4152,18 +4486,21 @@
         <v>0</v>
       </c>
       <c r="Y47">
+        <v>0</v>
+      </c>
+      <c r="Z47">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A48">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48">
         <v>47</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -4202,10 +4539,10 @@
         <v>0</v>
       </c>
       <c r="P48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48">
         <v>0</v>
@@ -4229,18 +4566,21 @@
         <v>0</v>
       </c>
       <c r="Y48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="Z48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49">
         <v>48</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -4252,11 +4592,11 @@
         <v>0</v>
       </c>
       <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
         <v>2</v>
       </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
       <c r="I49">
         <v>0</v>
       </c>
@@ -4288,10 +4628,10 @@
         <v>0</v>
       </c>
       <c r="S49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49">
         <v>0</v>
@@ -4306,18 +4646,21 @@
         <v>0</v>
       </c>
       <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A50">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50">
         <v>49</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -4338,10 +4681,10 @@
         <v>0</v>
       </c>
       <c r="J50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -4383,18 +4726,21 @@
         <v>0</v>
       </c>
       <c r="Y50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="Z50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51">
         <v>50</v>
       </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -4409,19 +4755,19 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
         <v>2</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
       <c r="K51">
         <v>0</v>
       </c>
       <c r="L51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M51">
         <v>2</v>
@@ -4430,7 +4776,7 @@
         <v>2</v>
       </c>
       <c r="O51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P51">
         <v>0</v>
@@ -4439,13 +4785,13 @@
         <v>0</v>
       </c>
       <c r="R51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S51">
         <v>1</v>
       </c>
       <c r="T51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51">
         <v>0</v>
@@ -4460,18 +4806,21 @@
         <v>0</v>
       </c>
       <c r="Y51">
+        <v>0</v>
+      </c>
+      <c r="Z51">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A52">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52">
         <v>51</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -4525,10 +4874,10 @@
         <v>0</v>
       </c>
       <c r="U52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W52">
         <v>0</v>
@@ -4537,18 +4886,21 @@
         <v>0</v>
       </c>
       <c r="Y52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="Z52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53">
         <v>52</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -4605,27 +4957,30 @@
         <v>0</v>
       </c>
       <c r="V53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X53">
         <v>0</v>
       </c>
       <c r="Y53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54">
         <v>53</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
       <c r="C54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -4664,10 +5019,10 @@
         <v>0</v>
       </c>
       <c r="P54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R54">
         <v>0</v>
@@ -4691,18 +5046,21 @@
         <v>0</v>
       </c>
       <c r="Y54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="Z54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55">
         <v>54</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -4756,10 +5114,10 @@
         <v>0</v>
       </c>
       <c r="U55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W55">
         <v>0</v>
@@ -4768,18 +5126,21 @@
         <v>0</v>
       </c>
       <c r="Y55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="Z55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56">
         <v>55</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4833,10 +5194,10 @@
         <v>0</v>
       </c>
       <c r="U56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W56">
         <v>0</v>
@@ -4845,18 +5206,21 @@
         <v>0</v>
       </c>
       <c r="Y56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="Z56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57">
         <v>56</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -4898,10 +5262,10 @@
         <v>0</v>
       </c>
       <c r="Q57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S57">
         <v>0</v>
@@ -4922,18 +5286,21 @@
         <v>0</v>
       </c>
       <c r="Y57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="Z57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58">
         <v>57</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4972,11 +5339,11 @@
         <v>0</v>
       </c>
       <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
         <v>2</v>
       </c>
-      <c r="Q58">
-        <v>0</v>
-      </c>
       <c r="R58">
         <v>0</v>
       </c>
@@ -4999,18 +5366,21 @@
         <v>0</v>
       </c>
       <c r="Y58">
+        <v>0</v>
+      </c>
+      <c r="Z58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A59">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59">
         <v>58</v>
       </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -5061,10 +5431,10 @@
         <v>0</v>
       </c>
       <c r="T59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V59">
         <v>0</v>
@@ -5076,18 +5446,21 @@
         <v>0</v>
       </c>
       <c r="Y59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="Z59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60">
         <v>59</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -5108,11 +5481,11 @@
         <v>0</v>
       </c>
       <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
         <v>2</v>
       </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
       <c r="L60">
         <v>0</v>
       </c>
@@ -5120,11 +5493,11 @@
         <v>0</v>
       </c>
       <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
         <v>2</v>
       </c>
-      <c r="O60">
-        <v>0</v>
-      </c>
       <c r="P60">
         <v>0</v>
       </c>
@@ -5153,18 +5526,21 @@
         <v>0</v>
       </c>
       <c r="Y60">
+        <v>0</v>
+      </c>
+      <c r="Z60">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A61">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61">
         <v>60</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -5221,27 +5597,30 @@
         <v>0</v>
       </c>
       <c r="V61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X61">
         <v>0</v>
       </c>
       <c r="Y61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="Z61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62">
         <v>61</v>
       </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -5280,10 +5659,10 @@
         <v>0</v>
       </c>
       <c r="P62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R62">
         <v>0</v>
@@ -5307,18 +5686,21 @@
         <v>0</v>
       </c>
       <c r="Y62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="Z62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63">
         <v>62</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -5327,7 +5709,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -5384,27 +5766,30 @@
         <v>1</v>
       </c>
       <c r="Y63">
+        <v>1</v>
+      </c>
+      <c r="Z63">
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A64">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64">
         <v>63</v>
       </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64">
         <v>1</v>
@@ -5461,6 +5846,9 @@
         <v>1</v>
       </c>
       <c r="Y64">
+        <v>1</v>
+      </c>
+      <c r="Z64">
         <v>19</v>
       </c>
     </row>

</xml_diff>